<commit_message>
final push from me. have fun whoever continues this project
</commit_message>
<xml_diff>
--- a/documentation/stage_logboek_Niek-Middel.xlsx
+++ b/documentation/stage_logboek_Niek-Middel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://horizoncollege-my.sharepoint.com/personal/f_t_j_beekman_horizoncollege_nl/Documents/backuplaptop/stagecoordinatie SD 2022-2023/BPV/BPV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\unity-games\unity_test2\unity_Arduino_controlled_world\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="11_B0BDC3FC223070D2C21197DD9475507217B0CECC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{931BFB92-B162-4D3C-B8FD-0403F3ACBFDE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BAA116-AC6D-4A35-BE16-85FD06EAFEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uren periode 1 en 2" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Naam student:</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>week 23</t>
+  </si>
+  <si>
+    <t>gewerkt aan de documentatie te verbeteren en in te voegen</t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,7 +482,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -763,20 +766,20 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -792,7 +795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.1" customHeight="1">
+    <row r="2" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -812,7 +815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.1" customHeight="1">
+    <row r="3" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -830,7 +833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.1" customHeight="1">
+    <row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -848,7 +851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.1" customHeight="1">
+    <row r="5" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -866,7 +869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.1" customHeight="1">
+    <row r="6" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -884,7 +887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.1" customHeight="1">
+    <row r="7" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
@@ -902,7 +905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.1" customHeight="1">
+    <row r="8" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -920,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.1" customHeight="1">
+    <row r="9" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -938,7 +941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.1" customHeight="1">
+    <row r="10" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -956,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.1" customHeight="1">
+    <row r="11" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -974,7 +977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.1" customHeight="1">
+    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -992,7 +995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.1" customHeight="1">
+    <row r="13" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.1" customHeight="1">
+    <row r="14" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.1" customHeight="1">
+    <row r="15" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.1" customHeight="1">
+    <row r="16" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.1" customHeight="1">
+    <row r="17" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.1" customHeight="1">
+    <row r="18" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.1" customHeight="1">
+    <row r="19" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.1" customHeight="1">
+    <row r="20" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.1" customHeight="1">
+    <row r="21" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.1" customHeight="1">
+    <row r="22" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
@@ -1172,26 +1175,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.1" customHeight="1">
+    <row r="23" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="7">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7">
+        <v>24</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="14.1" customHeight="1">
+      <c r="E23" s="23">
+        <v>24</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="22">
         <f>SUM(C3:C23)</f>
-        <v>630</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="14.1" customHeight="1">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>32</v>
       </c>
@@ -1200,11 +1211,11 @@
       <c r="D25" s="5"/>
       <c r="E25" s="24">
         <f>SUM(E3:E23)</f>
-        <v>630</v>
+        <v>654</v>
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1212,7 +1223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>35</v>
       </c>
@@ -1234,23 +1245,23 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="72.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="72.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="31"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -1258,7 +1269,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="3" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1277,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="4" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
@@ -1274,7 +1285,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="5" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
@@ -1282,7 +1293,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="6" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
@@ -1290,7 +1301,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="7" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>14</v>
       </c>
@@ -1298,7 +1309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>15</v>
       </c>
@@ -1306,7 +1317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="9" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>16</v>
       </c>
@@ -1314,7 +1325,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="10" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="11" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>18</v>
       </c>
@@ -1330,7 +1341,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="12" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>19</v>
       </c>
@@ -1338,7 +1349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="13" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>49</v>
       </c>
@@ -1346,7 +1357,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="14" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
@@ -1354,7 +1365,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="15" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
@@ -1362,7 +1373,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="16" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>23</v>
       </c>
@@ -1370,7 +1381,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="17" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>24</v>
       </c>
@@ -1378,7 +1389,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="18" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1386,7 +1397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="40.5" customHeight="1">
+    <row r="19" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>26</v>
       </c>
@@ -1394,7 +1405,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="20" spans="1:2" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1413,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="39" customHeight="1">
+    <row r="21" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1421,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="39" customHeight="1">
+    <row r="22" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>29</v>
       </c>
@@ -1418,19 +1429,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="39" customHeight="1">
+    <row r="23" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="20"/>
-    </row>
-    <row r="24" spans="1:2" ht="39" customHeight="1">
+      <c r="B23" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="20"/>
     </row>
-    <row r="25" spans="1:2" ht="39" customHeight="1">
+    <row r="25" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>59</v>
       </c>
@@ -1446,21 +1459,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BC85EBB2A370F4D9CB2278793666336" ma:contentTypeVersion="6" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="61a62ffaa98978017a2a8cf13a1f4ff3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="97b8365b-8efe-4081-b621-d4a5b4515a15" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2123d0bf18abcaf5bc8a520bb840435a" ns2:_="">
     <xsd:import namespace="97b8365b-8efe-4081-b621-d4a5b4515a15"/>
@@ -1618,14 +1616,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB31BCA6-79F9-4D98-B9FE-D2FAE076BADD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F079E8A3-E15B-4DA2-96BD-D28E7509D03F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="97b8365b-8efe-4081-b621-d4a5b4515a15"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13CF9906-8523-4196-8BBF-372D7C17BB60}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13CF9906-8523-4196-8BBF-372D7C17BB60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F079E8A3-E15B-4DA2-96BD-D28E7509D03F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB31BCA6-79F9-4D98-B9FE-D2FAE076BADD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>